<commit_message>
Update census data and revise component definitions
Updated multiple disability_prevalence.xlsx files across regions with new data. Added new data files for javaxeti municipalities, including age dependency, wages, education, healthcare staff, and population totals. Revised components.csv to simplify and clarify component descriptions. Updated municipalities.csv to adjust region codes for javaxeti, racha, and tbilisi.
</commit_message>
<xml_diff>
--- a/data/georgia_census/adjara/batumi/disability_prevalence.xlsx
+++ b/data/georgia_census/adjara/batumi/disability_prevalence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\შშმ პირები სრული\დევნილი შშმ პირები ქარ. EN\მუნიციპალიტეტი\EN\Adjara A. R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\შშმ პირები სრული\სოც. დახ. ბაზ. რეგ. შშმ პირები ქარ. EN\მუნიციპალიტეტი\EN\Adjara A. R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD641AB-6D18-4EB3-A726-80A3F35B7CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F26E40-555A-4DEA-AA5D-4D9A050E0F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5A32126C-9B11-445B-BA17-94C72F9786C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{678E4DE4-C647-44FA-920F-70F3C188BA9A}"/>
   </bookViews>
   <sheets>
     <sheet name="C.Batumi" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>(End of year, persons)</t>
-  </si>
-  <si>
-    <t>Number of disability persons</t>
   </si>
   <si>
     <r>
@@ -55,17 +52,24 @@
     </r>
   </si>
   <si>
-    <t>Number of Internally Displaced Disability Persons Receiving Social Package in C. Batumi Municipality</t>
+    <t xml:space="preserve">family with disabilities Persons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">disabilities Persons </t>
+  </si>
+  <si>
+    <t>The number of persons with disabilities registered in the Unified database of targeted social assistance program in C. Batumi Municipality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#\ ##0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +78,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
@@ -81,12 +102,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -102,12 +117,6 @@
       <u/>
       <sz val="9"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -126,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -154,36 +163,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{BEF522A9-2AD6-4DAD-A8C1-52B78F158236}"/>
+    <cellStyle name="Comma 3" xfId="4" xr:uid="{E298EC3B-CB9A-4AB6-ABFF-F968FEA4E95B}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_01_IANVARI" xfId="1" xr:uid="{6F131FFA-B50B-4D9F-BD69-276859E625FE}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{427CB489-A07A-4491-B59E-A7C501DA5D05}"/>
+    <cellStyle name="Normal_01_IANVARI" xfId="2" xr:uid="{4B9A7469-AC35-48FB-8CC2-8E7BD64B8A63}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -494,32 +522,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D3897C-AD82-4D74-A40C-FD3DBD2FEBFB}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9B46AF-A91B-4475-9DA7-525AD3351F02}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="1" customWidth="1"/>
-    <col min="2" max="8" width="7.6328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6328125" customWidth="1"/>
-    <col min="10" max="16" width="7.6328125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="20.81640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>3</v>
-      </c>
+    <row r="1" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
       <c r="B3" s="2">
         <v>2017</v>
       </c>
@@ -545,50 +579,80 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1446</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1458</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1501</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1682</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1813</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1970</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2082</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1678</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1692</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1731</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1932</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2071</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2249</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2397</v>
+      </c>
+      <c r="I5" s="11">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
-        <v>80</v>
-      </c>
-      <c r="C4" s="3">
-        <v>75</v>
-      </c>
-      <c r="D4" s="4">
-        <v>78</v>
-      </c>
-      <c r="E4" s="4">
-        <v>73</v>
-      </c>
-      <c r="F4" s="4">
-        <v>65</v>
-      </c>
-      <c r="G4" s="4">
-        <v>121</v>
-      </c>
-      <c r="H4" s="4">
-        <v>114</v>
-      </c>
-      <c r="I4" s="4">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A5:H5"/>
+  <mergeCells count="2">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>